<commit_message>
added some more scripts
</commit_message>
<xml_diff>
--- a/phillips_COT_data.xlsx
+++ b/phillips_COT_data.xlsx
@@ -336,13 +336,14 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D30" activeCellId="0" sqref="D30"/>
+      <selection pane="topRight" activeCell="F33" activeCellId="0" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.24"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3900,7 +3901,7 @@
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.39"/>
@@ -4742,7 +4743,7 @@
       <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5107,7 +5108,7 @@
       <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>